<commit_message>
PageObjects added for Add, Enter new application and View/Edit visitors list pages.
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/testInput.xlsx
+++ b/src/test/resources/inputFiles/testInput.xlsx
@@ -25,10 +25,10 @@
     <t xml:space="preserve">brandNewVisitorEmailId</t>
   </si>
   <si>
-    <t xml:space="preserve">test6767@gmail.com</t>
+    <t>SeleniumTest+v20190913120541@gmail.com</t>
   </si>
   <si>
-    <t>ajay.rsin@gmail.com</t>
+    <t>SeleniumTest+v20190913120708@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -38,7 +38,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -59,13 +59,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -110,12 +103,8 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -136,7 +125,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -153,20 +142,17 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
-      <c r="A2" s="1" t="s">
+    <row r="2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="B3" t="s">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink display="test6767@gmail.com" r:id="rId1" ref="A2"/>
-  </hyperlinks>
   <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>

</xml_diff>

<commit_message>
Minor changes to the architecture diagram in read me file.
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/testInput.xlsx
+++ b/src/test/resources/inputFiles/testInput.xlsx
@@ -25,10 +25,10 @@
     <t xml:space="preserve">brandNewVisitorEmailId</t>
   </si>
   <si>
-    <t>SeleniumTest+v20190918155235@gmail.com</t>
+    <t>SeleniumTest+v20190923115753@gmail.com</t>
   </si>
   <si>
-    <t>SeleniumTest+v20190918155403@gmail.com</t>
+    <t>SeleniumTest+v20190923115921@gmail.com</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
changed the executionReports directory path to resources folder.
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/testInput.xlsx
+++ b/src/test/resources/inputFiles/testInput.xlsx
@@ -25,10 +25,10 @@
     <t xml:space="preserve">brandNewVisitorEmailId</t>
   </si>
   <si>
-    <t>SeleniumTest+v20190923115753@gmail.com</t>
+    <t>SeleniumTest+v20191001121230@gmail.com</t>
   </si>
   <si>
-    <t>SeleniumTest+v20190923115921@gmail.com</t>
+    <t>SeleniumTest+v20191001121358@gmail.com</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Started to change the login logic. Yet to complete, In progress.
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/testInput.xlsx
+++ b/src/test/resources/inputFiles/testInput.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" date1904="false" showObjects="all"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="addVisitor" r:id="rId2" sheetId="1" state="visible"/>
+    <sheet name="addVisitor" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterate="false" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,15 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t xml:space="preserve">brandNewVisitorEmailId</t>
-  </si>
-  <si>
-    <t>SeleniumTest+v20191001121230@gmail.com</t>
-  </si>
-  <si>
-    <t>SeleniumTest+v20191001121358@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -70,7 +64,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -79,43 +73,43 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -125,37 +119,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="20.6" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.6"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Introduced setup script for the pack, this will clear the testinput.xlsx file.
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/testInput.xlsx
+++ b/src/test/resources/inputFiles/testInput.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" date1904="false" showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="addVisitor" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="addVisitor" r:id="rId2" sheetId="1" state="visible"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterate="false" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,9 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">brandNewVisitorEmailId</t>
+  </si>
+  <si>
+    <t>SeleniumTest+v20191015125116@gmail.com</t>
+  </si>
+  <si>
+    <t>SeleniumTest+v20191015125425@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -64,7 +70,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -73,43 +79,43 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -119,27 +125,41 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.6"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="20.6" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5"/>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
included sql property file and excel sheet for sql row and column count.
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/testInput.xlsx
+++ b/src/test/resources/inputFiles/testInput.xlsx
@@ -20,18 +20,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t xml:space="preserve">brandNewVisitorEmailId</t>
   </si>
   <si>
-    <t xml:space="preserve">SeleniumTest+v20191015142109@gmail.com</t>
+    <t xml:space="preserve">sqlRecordCount</t>
   </si>
   <si>
-    <t>SeleniumTest+v20191015144231@gmail.com</t>
+    <t xml:space="preserve">sqlColCount</t>
   </si>
   <si>
-    <t>SeleniumTest+v20191015144444@gmail.com</t>
+    <t xml:space="preserve">252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t>252</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -128,7 +140,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -137,26 +149,30 @@
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
   <cols>
     <col min="1" max="1" customWidth="true" hidden="false" style="0" width="20.6" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="14.35" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5"/>
-    <row r="6">
-      <c r="A6" t="s">
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>3</v>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created new sheet for sqlCount.
</commit_message>
<xml_diff>
--- a/src/test/resources/inputFiles/testInput.xlsx
+++ b/src/test/resources/inputFiles/testInput.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="addVisitor" r:id="rId2" sheetId="1" state="visible"/>
+    <sheet name="sqlCount" r:id="rId3" sheetId="2" state="visible"/>
   </sheets>
   <calcPr iterate="false" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">brandNewVisitorEmailId</t>
   </si>
@@ -31,16 +32,13 @@
     <t xml:space="preserve">sqlColCount</t>
   </si>
   <si>
-    <t xml:space="preserve">252</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
+    <t>SeleniumTest+v20191017153943@gmail.com</t>
+  </si>
+  <si>
+    <t>SeleniumTest+v20191017154305@gmail.com</t>
   </si>
   <si>
     <t>252</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
   <si>
     <t>5</t>
@@ -140,7 +138,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -157,22 +155,59 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0" zeroHeight="false"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="14.35" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="s">
+        <v>1</v>
+      </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
-      <c r="A2" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="B2" s="0" t="s">
+    <row r="2">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>7</v>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>